<commit_message>
Update lambert functions (#121)
* add lambert tmax_rp function + tests

* update lambert battin function/tests

* update spreadsheet

* update spreadsheet
</commit_message>
<xml_diff>
--- a/Astro Software.xlsx
+++ b/Astro Software.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Software" sheetId="1" state="visible" r:id="rId3"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2803" uniqueCount="1473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2805" uniqueCount="1475">
   <si>
     <t xml:space="preserve">Astrodynamics Software </t>
   </si>
@@ -3730,46 +3730,52 @@
     <t xml:space="preserve">anglesdr</t>
   </si>
   <si>
-    <t xml:space="preserve">valladopy.astro.twobody.lambert.min_energy</t>
+    <t xml:space="preserve">valladopy.astro.iod.lambert.min_energy</t>
   </si>
   <si>
     <t xml:space="preserve">lambertmin</t>
   </si>
   <si>
-    <t xml:space="preserve">valladopy.astro.twobody.lambert.min_time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">valladopy.astro.twobody.lambert.seebatt</t>
+    <t xml:space="preserve">valladopy.astro.iod.lambert.min_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.astro.iod.lambert.tmax_rp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lamberttmaxrp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.astro.iod.lambert.seebatt</t>
   </si>
   <si>
     <t xml:space="preserve">seebatt</t>
   </si>
   <si>
-    <t xml:space="preserve">valladopy.astro.twobody.lambert.kbatt</t>
+    <t xml:space="preserve">valladopy.astro.iod.lambert.kbatt</t>
   </si>
   <si>
     <t xml:space="preserve">kbatt</t>
   </si>
   <si>
-    <t xml:space="preserve">valladopy.astro.twobody.lambert.hodograph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">valladopy.astro.twobody.lambert.battin</t>
+    <t xml:space="preserve">valladopy.astro.iod.lambert.hodograph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.astro.iod.lambert.battin</t>
   </si>
   <si>
     <t xml:space="preserve">lambertb</t>
   </si>
   <si>
-    <t xml:space="preserve">valladopy.astro.twobody.lambert.get_tbiu</t>
+    <t xml:space="preserve">valladopy.astro.iod.lambert.get_tbiu</t>
   </si>
   <si>
     <t xml:space="preserve">lambgetbiu</t>
   </si>
   <si>
-    <t xml:space="preserve">valladopy.astro.twobody.lambert.universal_min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">valladopy.astro.twobody.lambert.universal</t>
+    <t xml:space="preserve">valladopy.astro.iod.lambert.universal_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.astro.iod.lambert.universal</t>
   </si>
   <si>
     <t xml:space="preserve">lambertu</t>
@@ -4647,7 +4653,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d\-mmm"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -4783,6 +4789,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4924,7 +4936,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5113,6 +5125,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5125,7 +5141,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5383,10 +5399,10 @@
   </sheetPr>
   <dimension ref="A1:P344"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="7" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="7" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H83" activeCellId="0" sqref="H83"/>
+      <selection pane="bottomLeft" activeCell="I194" activeCellId="0" sqref="I194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="11.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9079,7 +9095,7 @@
       <c r="D195" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F195" s="7" t="s">
+      <c r="F195" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J195" s="2" t="s">
@@ -15881,10 +15897,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB1040"/>
+  <dimension ref="A1:AB1041"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A127" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E149" activeCellId="0" sqref="E149"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16143,10 +16159,10 @@
         <v>338</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="41"/>
       <c r="B21" s="41"/>
-      <c r="C21" s="43" t="s">
+      <c r="C21" s="47" t="s">
         <v>1173</v>
       </c>
       <c r="D21" s="44" t="s">
@@ -16170,17 +16186,17 @@
         <v>1177</v>
       </c>
       <c r="D23" s="44" t="s">
-        <v>344</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="41"/>
       <c r="B24" s="41"/>
       <c r="C24" s="43" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="D24" s="44" t="s">
-        <v>1179</v>
+        <v>344</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16200,17 +16216,17 @@
         <v>1182</v>
       </c>
       <c r="D26" s="44" t="s">
-        <v>336</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="41"/>
       <c r="B27" s="41"/>
       <c r="C27" s="43" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="D27" s="44" t="s">
-        <v>1184</v>
+        <v>336</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16220,42 +16236,42 @@
         <v>1185</v>
       </c>
       <c r="D28" s="44" t="s">
-        <v>371</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="41"/>
       <c r="B29" s="41"/>
-      <c r="C29" s="45" t="s">
-        <v>1186</v>
-      </c>
-      <c r="D29" s="46" t="s">
+      <c r="C29" s="43" t="s">
         <v>1187</v>
       </c>
-      <c r="E29" s="45"/>
+      <c r="D29" s="44" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="41"/>
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="41"/>
+      <c r="C30" s="45" t="s">
         <v>1188</v>
       </c>
-      <c r="C30" s="43" t="s">
+      <c r="D30" s="46" t="s">
         <v>1189</v>
       </c>
-      <c r="D30" s="44" t="s">
-        <v>1190</v>
-      </c>
-      <c r="E30" s="43" t="s">
-        <v>1191</v>
-      </c>
+      <c r="E30" s="45"/>
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="41"/>
-      <c r="B31" s="41"/>
+      <c r="B31" s="41" t="s">
+        <v>1190</v>
+      </c>
       <c r="C31" s="43" t="s">
+        <v>1191</v>
+      </c>
+      <c r="D31" s="44" t="s">
         <v>1192</v>
       </c>
-      <c r="D31" s="44" t="s">
+      <c r="E31" s="43" t="s">
         <v>1193</v>
       </c>
     </row>
@@ -16352,174 +16368,171 @@
     <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="41"/>
       <c r="B41" s="41"/>
-      <c r="C41" s="45" t="s">
+      <c r="C41" s="43" t="s">
         <v>1212</v>
       </c>
-      <c r="D41" s="46" t="s">
+      <c r="D41" s="44" t="s">
         <v>1213</v>
       </c>
-      <c r="E41" s="45"/>
     </row>
     <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="41"/>
-      <c r="B42" s="41" t="s">
+      <c r="B42" s="41"/>
+      <c r="C42" s="45" t="s">
         <v>1214</v>
       </c>
-      <c r="C42" s="43" t="s">
+      <c r="D42" s="46" t="s">
         <v>1215</v>
       </c>
-      <c r="D42" s="44" t="s">
-        <v>1007</v>
-      </c>
+      <c r="E42" s="45"/>
     </row>
     <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="B43" s="41" t="s">
+        <v>1216</v>
+      </c>
       <c r="C43" s="43" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="D43" s="44" t="s">
-        <v>415</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="41"/>
       <c r="B44" s="41"/>
-      <c r="C44" s="45" t="s">
-        <v>1217</v>
-      </c>
-      <c r="D44" s="46" t="s">
+      <c r="C44" s="43" t="s">
         <v>1218</v>
       </c>
-      <c r="E44" s="45"/>
+      <c r="D44" s="44" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="41"/>
-      <c r="B45" s="41" t="s">
+      <c r="B45" s="41"/>
+      <c r="C45" s="45" t="s">
         <v>1219</v>
       </c>
-      <c r="C45" s="43" t="s">
+      <c r="D45" s="46" t="s">
         <v>1220</v>
       </c>
-      <c r="D45" s="44" t="s">
-        <v>545</v>
-      </c>
+      <c r="E45" s="45"/>
     </row>
     <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="41"/>
-      <c r="B46" s="41"/>
+      <c r="B46" s="41" t="s">
+        <v>1221</v>
+      </c>
       <c r="C46" s="43" t="s">
-        <v>1221</v>
-      </c>
-      <c r="D46" s="46" t="s">
         <v>1222</v>
       </c>
-      <c r="E46" s="45"/>
+      <c r="D46" s="44" t="s">
+        <v>545</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="41"/>
-      <c r="B47" s="41" t="s">
+      <c r="B47" s="41"/>
+      <c r="C47" s="43" t="s">
         <v>1223</v>
       </c>
-      <c r="C47" s="47" t="s">
+      <c r="D47" s="46" t="s">
         <v>1224</v>
       </c>
-      <c r="D47" s="44" t="s">
-        <v>1225</v>
-      </c>
-      <c r="E47" s="43" t="s">
-        <v>1226</v>
-      </c>
+      <c r="E47" s="45"/>
     </row>
     <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="41"/>
-      <c r="B48" s="41"/>
-      <c r="C48" s="43" t="s">
+      <c r="B48" s="41" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C48" s="48" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D48" s="44" t="s">
         <v>1227</v>
       </c>
-      <c r="D48" s="44" t="s">
+      <c r="E48" s="43" t="s">
         <v>1228</v>
-      </c>
-      <c r="E48" s="43" t="s">
-        <v>1229</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="41"/>
       <c r="B49" s="41"/>
-      <c r="C49" s="45" t="s">
+      <c r="C49" s="43" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D49" s="44" t="s">
         <v>1230</v>
       </c>
-      <c r="D49" s="46" t="s">
-        <v>391</v>
-      </c>
-      <c r="E49" s="45"/>
+      <c r="E49" s="43" t="s">
+        <v>1231</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="41"/>
-      <c r="B50" s="41" t="s">
-        <v>1231</v>
-      </c>
-      <c r="C50" s="43" t="s">
+      <c r="B50" s="41"/>
+      <c r="C50" s="45" t="s">
         <v>1232</v>
       </c>
-      <c r="D50" s="44" t="s">
-        <v>476</v>
-      </c>
-      <c r="E50" s="43" t="s">
-        <v>1233</v>
-      </c>
+      <c r="D50" s="46" t="s">
+        <v>391</v>
+      </c>
+      <c r="E50" s="45"/>
     </row>
     <row r="51" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="41"/>
-      <c r="B51" s="41"/>
+      <c r="B51" s="41" t="s">
+        <v>1233</v>
+      </c>
       <c r="C51" s="43" t="s">
         <v>1234</v>
       </c>
       <c r="D51" s="44" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="E51" s="43" t="s">
-        <v>1233</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="41"/>
       <c r="B52" s="41"/>
       <c r="C52" s="43" t="s">
+        <v>1236</v>
+      </c>
+      <c r="D52" s="44" t="s">
+        <v>474</v>
+      </c>
+      <c r="E52" s="43" t="s">
         <v>1235</v>
-      </c>
-      <c r="D52" s="44" t="s">
-        <v>470</v>
-      </c>
-      <c r="E52" s="43" t="s">
-        <v>1233</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="41"/>
       <c r="B53" s="41"/>
       <c r="C53" s="43" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="D53" s="44" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="E53" s="43" t="s">
-        <v>1233</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="41"/>
       <c r="B54" s="41"/>
       <c r="C54" s="43" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="D54" s="44" t="s">
-        <v>485</v>
+        <v>472</v>
       </c>
       <c r="E54" s="43" t="s">
-        <v>1238</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16529,144 +16542,144 @@
         <v>1239</v>
       </c>
       <c r="D55" s="44" t="s">
-        <v>468</v>
+        <v>485</v>
       </c>
       <c r="E55" s="43" t="s">
-        <v>1238</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="41"/>
       <c r="B56" s="41"/>
       <c r="C56" s="43" t="s">
+        <v>1241</v>
+      </c>
+      <c r="D56" s="44" t="s">
+        <v>468</v>
+      </c>
+      <c r="E56" s="43" t="s">
         <v>1240</v>
-      </c>
-      <c r="D56" s="44" t="s">
-        <v>478</v>
-      </c>
-      <c r="E56" s="43" t="s">
-        <v>1238</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="41"/>
       <c r="B57" s="41"/>
       <c r="C57" s="43" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="D57" s="44" t="s">
-        <v>1231</v>
+        <v>478</v>
       </c>
       <c r="E57" s="43" t="s">
-        <v>1238</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="41"/>
       <c r="B58" s="41"/>
-      <c r="C58" s="45" t="s">
-        <v>1242</v>
-      </c>
-      <c r="D58" s="46" t="s">
-        <v>482</v>
-      </c>
-      <c r="E58" s="45"/>
+      <c r="C58" s="43" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D58" s="44" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E58" s="43" t="s">
+        <v>1240</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="41"/>
-      <c r="B59" s="41" t="s">
-        <v>1243</v>
-      </c>
-      <c r="C59" s="43" t="s">
+      <c r="B59" s="41"/>
+      <c r="C59" s="45" t="s">
         <v>1244</v>
       </c>
-      <c r="D59" s="44" t="s">
-        <v>458</v>
-      </c>
+      <c r="D59" s="46" t="s">
+        <v>482</v>
+      </c>
+      <c r="E59" s="45"/>
     </row>
     <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="41"/>
-      <c r="B60" s="41"/>
+      <c r="B60" s="41" t="s">
+        <v>1245</v>
+      </c>
       <c r="C60" s="43" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="D60" s="44" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="41"/>
       <c r="B61" s="41"/>
       <c r="C61" s="43" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="D61" s="44" t="s">
-        <v>232</v>
+        <v>459</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="41"/>
       <c r="B62" s="41"/>
       <c r="C62" s="43" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="D62" s="44" t="s">
-        <v>460</v>
+        <v>232</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="41"/>
       <c r="B63" s="41"/>
       <c r="C63" s="43" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="D63" s="44" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="41"/>
       <c r="B64" s="41"/>
       <c r="C64" s="43" t="s">
-        <v>1249</v>
-      </c>
-      <c r="D64" s="48" t="s">
         <v>1250</v>
       </c>
-      <c r="E64" s="49" t="s">
-        <v>1251</v>
+      <c r="D64" s="44" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="41"/>
       <c r="B65" s="41"/>
       <c r="C65" s="43" t="s">
+        <v>1251</v>
+      </c>
+      <c r="D65" s="49" t="s">
         <v>1252</v>
       </c>
-      <c r="D65" s="48"/>
-      <c r="E65" s="48"/>
+      <c r="E65" s="50" t="s">
+        <v>1253</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="41"/>
       <c r="B66" s="41"/>
       <c r="C66" s="43" t="s">
-        <v>1253</v>
-      </c>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
+        <v>1254</v>
+      </c>
+      <c r="D66" s="49"/>
+      <c r="E66" s="49"/>
     </row>
     <row r="67" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="41"/>
       <c r="B67" s="41"/>
       <c r="C67" s="43" t="s">
-        <v>1254</v>
-      </c>
-      <c r="D67" s="48" t="s">
         <v>1255</v>
       </c>
-      <c r="E67" s="49" t="s">
-        <v>1251</v>
-      </c>
+      <c r="D67" s="49"/>
+      <c r="E67" s="49"/>
     </row>
     <row r="68" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="41"/>
@@ -16674,36 +16687,39 @@
       <c r="C68" s="43" t="s">
         <v>1256</v>
       </c>
-      <c r="D68" s="48"/>
-      <c r="E68" s="48"/>
+      <c r="D68" s="49" t="s">
+        <v>1257</v>
+      </c>
+      <c r="E68" s="50" t="s">
+        <v>1253</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="41"/>
       <c r="B69" s="41"/>
       <c r="C69" s="43" t="s">
-        <v>1257</v>
-      </c>
-      <c r="D69" s="48"/>
-      <c r="E69" s="48"/>
+        <v>1258</v>
+      </c>
+      <c r="D69" s="49"/>
+      <c r="E69" s="49"/>
     </row>
     <row r="70" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="41"/>
       <c r="B70" s="41"/>
       <c r="C70" s="43" t="s">
-        <v>1258</v>
-      </c>
-      <c r="D70" s="48"/>
-      <c r="E70" s="48"/>
+        <v>1259</v>
+      </c>
+      <c r="D70" s="49"/>
+      <c r="E70" s="49"/>
     </row>
     <row r="71" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="41"/>
       <c r="B71" s="41"/>
       <c r="C71" s="43" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D71" s="44" t="s">
         <v>1260</v>
       </c>
+      <c r="D71" s="49"/>
+      <c r="E71" s="49"/>
     </row>
     <row r="72" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="41"/>
@@ -16992,17 +17008,17 @@
         <v>1317</v>
       </c>
       <c r="D100" s="44" t="s">
-        <v>219</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="41"/>
       <c r="B101" s="41"/>
       <c r="C101" s="43" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="D101" s="44" t="s">
-        <v>1319</v>
+        <v>219</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17022,67 +17038,67 @@
         <v>1322</v>
       </c>
       <c r="D103" s="44" t="s">
-        <v>233</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="41"/>
       <c r="B104" s="41"/>
       <c r="C104" s="43" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="D104" s="44" t="s">
-        <v>962</v>
+        <v>233</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="41"/>
       <c r="B105" s="41"/>
       <c r="C105" s="43" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="D105" s="44" t="s">
-        <v>227</v>
+        <v>962</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="41"/>
       <c r="B106" s="41"/>
       <c r="C106" s="43" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="D106" s="44" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="41"/>
       <c r="B107" s="41"/>
       <c r="C107" s="43" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="D107" s="44" t="s">
-        <v>461</v>
+        <v>229</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="41"/>
       <c r="B108" s="41"/>
       <c r="C108" s="43" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="D108" s="44" t="s">
-        <v>961</v>
+        <v>461</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="41"/>
       <c r="B109" s="41"/>
       <c r="C109" s="43" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="D109" s="44" t="s">
-        <v>1329</v>
+        <v>961</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17092,120 +17108,119 @@
         <v>1330</v>
       </c>
       <c r="D110" s="44" t="s">
-        <v>223</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="41"/>
       <c r="B111" s="41"/>
       <c r="C111" s="43" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="D111" s="44" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="41"/>
       <c r="B112" s="41"/>
       <c r="C112" s="43" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="D112" s="44" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="41"/>
       <c r="B113" s="41"/>
       <c r="C113" s="43" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="D113" s="44" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="41"/>
       <c r="B114" s="41"/>
       <c r="C114" s="43" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="D114" s="44" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="41"/>
       <c r="B115" s="41"/>
       <c r="C115" s="43" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="D115" s="44" t="s">
-        <v>465</v>
-      </c>
-      <c r="E115" s="43" t="s">
-        <v>1336</v>
+        <v>239</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="41"/>
       <c r="B116" s="41"/>
-      <c r="C116" s="45" t="s">
+      <c r="C116" s="43" t="s">
         <v>1337</v>
       </c>
-      <c r="D116" s="46" t="s">
-        <v>464</v>
-      </c>
-      <c r="E116" s="45"/>
+      <c r="D116" s="44" t="s">
+        <v>465</v>
+      </c>
+      <c r="E116" s="43" t="s">
+        <v>1338</v>
+      </c>
     </row>
     <row r="117" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="41"/>
-      <c r="B117" s="41" t="s">
-        <v>1338</v>
-      </c>
-      <c r="C117" s="43" t="s">
+      <c r="B117" s="41"/>
+      <c r="C117" s="45" t="s">
         <v>1339</v>
       </c>
-      <c r="D117" s="44" t="s">
-        <v>1340</v>
-      </c>
-      <c r="E117" s="43" t="s">
-        <v>1341</v>
-      </c>
+      <c r="D117" s="46" t="s">
+        <v>464</v>
+      </c>
+      <c r="E117" s="45"/>
     </row>
     <row r="118" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="41"/>
-      <c r="B118" s="41"/>
+      <c r="B118" s="41" t="s">
+        <v>1340</v>
+      </c>
       <c r="C118" s="43" t="s">
+        <v>1341</v>
+      </c>
+      <c r="D118" s="44" t="s">
         <v>1342</v>
       </c>
-      <c r="D118" s="44" t="s">
+      <c r="E118" s="43" t="s">
         <v>1343</v>
-      </c>
-      <c r="E118" s="43" t="s">
-        <v>1344</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="41"/>
       <c r="B119" s="41"/>
       <c r="C119" s="43" t="s">
+        <v>1344</v>
+      </c>
+      <c r="D119" s="44" t="s">
         <v>1345</v>
       </c>
-      <c r="D119" s="44" t="s">
-        <v>428</v>
-      </c>
-      <c r="E119" s="43"/>
+      <c r="E119" s="43" t="s">
+        <v>1346</v>
+      </c>
     </row>
     <row r="120" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="41"/>
       <c r="B120" s="41"/>
       <c r="C120" s="43" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="D120" s="44" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E120" s="43"/>
     </row>
@@ -17213,10 +17228,10 @@
       <c r="A121" s="41"/>
       <c r="B121" s="41"/>
       <c r="C121" s="43" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="D121" s="44" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E121" s="43"/>
     </row>
@@ -17224,10 +17239,10 @@
       <c r="A122" s="41"/>
       <c r="B122" s="41"/>
       <c r="C122" s="43" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="D122" s="44" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E122" s="43"/>
     </row>
@@ -17235,10 +17250,10 @@
       <c r="A123" s="41"/>
       <c r="B123" s="41"/>
       <c r="C123" s="43" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="D123" s="44" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E123" s="43"/>
     </row>
@@ -17246,10 +17261,10 @@
       <c r="A124" s="41"/>
       <c r="B124" s="41"/>
       <c r="C124" s="43" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="D124" s="44" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E124" s="43"/>
     </row>
@@ -17257,10 +17272,10 @@
       <c r="A125" s="41"/>
       <c r="B125" s="41"/>
       <c r="C125" s="43" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="D125" s="44" t="s">
-        <v>1352</v>
+        <v>438</v>
       </c>
       <c r="E125" s="43"/>
     </row>
@@ -17282,7 +17297,7 @@
         <v>1355</v>
       </c>
       <c r="D127" s="44" t="s">
-        <v>420</v>
+        <v>1356</v>
       </c>
       <c r="E127" s="43"/>
     </row>
@@ -17290,10 +17305,10 @@
       <c r="A128" s="41"/>
       <c r="B128" s="41"/>
       <c r="C128" s="43" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="D128" s="44" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="E128" s="43"/>
     </row>
@@ -17301,83 +17316,84 @@
       <c r="A129" s="41"/>
       <c r="B129" s="41"/>
       <c r="C129" s="43" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="D129" s="44" t="s">
-        <v>1358</v>
-      </c>
-      <c r="E129" s="43" t="s">
-        <v>1359</v>
-      </c>
+        <v>418</v>
+      </c>
+      <c r="E129" s="43"/>
     </row>
     <row r="130" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="41"/>
       <c r="B130" s="41"/>
       <c r="C130" s="43" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D130" s="44" t="s">
         <v>1360</v>
       </c>
-      <c r="D130" s="44" t="s">
-        <v>287</v>
+      <c r="E130" s="43" t="s">
+        <v>1361</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="41"/>
       <c r="B131" s="41"/>
       <c r="C131" s="43" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D131" s="44" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="41"/>
       <c r="B132" s="41"/>
       <c r="C132" s="43" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="D132" s="44" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="41"/>
       <c r="B133" s="41"/>
       <c r="C133" s="43" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="D133" s="44" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="41"/>
       <c r="B134" s="41"/>
       <c r="C134" s="43" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="D134" s="44" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="41"/>
       <c r="B135" s="41"/>
       <c r="C135" s="43" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="D135" s="44" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="41"/>
       <c r="B136" s="41"/>
       <c r="C136" s="43" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="D136" s="44" t="s">
-        <v>1367</v>
+        <v>277</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17389,38 +17405,38 @@
       <c r="D137" s="44" t="s">
         <v>1369</v>
       </c>
-      <c r="E137" s="43" t="s">
-        <v>1370</v>
-      </c>
     </row>
     <row r="138" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="41"/>
       <c r="B138" s="41"/>
       <c r="C138" s="43" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D138" s="44" t="s">
         <v>1371</v>
       </c>
-      <c r="D138" s="44" t="s">
-        <v>283</v>
+      <c r="E138" s="43" t="s">
+        <v>1372</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="41"/>
       <c r="B139" s="41"/>
       <c r="C139" s="43" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="D139" s="44" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="41"/>
       <c r="B140" s="41"/>
       <c r="C140" s="43" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="D140" s="44" t="s">
-        <v>1374</v>
+        <v>281</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17472,17 +17488,17 @@
       <c r="D145" s="44" t="s">
         <v>1384</v>
       </c>
-      <c r="E145" s="50" t="s">
-        <v>1385</v>
-      </c>
     </row>
     <row r="146" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="41"/>
       <c r="B146" s="41"/>
       <c r="C146" s="43" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D146" s="44" t="s">
         <v>1386</v>
       </c>
-      <c r="D146" s="44" t="s">
+      <c r="E146" s="51" t="s">
         <v>1387</v>
       </c>
     </row>
@@ -17515,48 +17531,48 @@
       <c r="D149" s="44" t="s">
         <v>1393</v>
       </c>
-      <c r="E149" s="50" t="s">
-        <v>1394</v>
-      </c>
     </row>
     <row r="150" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="41"/>
       <c r="B150" s="41"/>
       <c r="C150" s="43" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D150" s="44" t="s">
         <v>1395</v>
       </c>
-      <c r="D150" s="44" t="s">
-        <v>305</v>
+      <c r="E150" s="51" t="s">
+        <v>1396</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="41"/>
       <c r="B151" s="41"/>
       <c r="C151" s="43" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="D151" s="44" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="41"/>
       <c r="B152" s="41"/>
       <c r="C152" s="43" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="D152" s="44" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="41"/>
       <c r="B153" s="41"/>
       <c r="C153" s="43" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="D153" s="44" t="s">
-        <v>1399</v>
+        <v>309</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17578,61 +17594,61 @@
       <c r="D155" s="44" t="s">
         <v>1403</v>
       </c>
-      <c r="E155" s="43" t="s">
-        <v>1404</v>
-      </c>
     </row>
     <row r="156" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="41"/>
       <c r="B156" s="41"/>
       <c r="C156" s="43" t="s">
+        <v>1404</v>
+      </c>
+      <c r="D156" s="44" t="s">
         <v>1405</v>
       </c>
-      <c r="D156" s="44" t="s">
+      <c r="E156" s="43" t="s">
         <v>1406</v>
-      </c>
-      <c r="E156" s="43" t="s">
-        <v>1407</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="41"/>
       <c r="B157" s="41"/>
       <c r="C157" s="43" t="s">
+        <v>1407</v>
+      </c>
+      <c r="D157" s="44" t="s">
         <v>1408</v>
       </c>
-      <c r="D157" s="44" t="s">
-        <v>985</v>
+      <c r="E157" s="43" t="s">
+        <v>1409</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="41"/>
       <c r="B158" s="41"/>
       <c r="C158" s="43" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="D158" s="44" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="41"/>
       <c r="B159" s="41"/>
       <c r="C159" s="43" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="D159" s="44" t="s">
-        <v>324</v>
+        <v>986</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="41"/>
       <c r="B160" s="41"/>
       <c r="C160" s="43" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="D160" s="44" t="s">
-        <v>1412</v>
+        <v>324</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17652,47 +17668,47 @@
         <v>1415</v>
       </c>
       <c r="D162" s="44" t="s">
-        <v>978</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="41"/>
       <c r="B163" s="41"/>
       <c r="C163" s="43" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="D163" s="44" t="s">
-        <v>974</v>
+        <v>978</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="41"/>
       <c r="B164" s="41"/>
       <c r="C164" s="43" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="D164" s="44" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="41"/>
       <c r="B165" s="41"/>
       <c r="C165" s="43" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="D165" s="44" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="41"/>
       <c r="B166" s="41"/>
       <c r="C166" s="43" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="D166" s="44" t="s">
-        <v>1420</v>
+        <v>976</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17722,37 +17738,37 @@
         <v>1425</v>
       </c>
       <c r="D169" s="44" t="s">
-        <v>353</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="41"/>
       <c r="B170" s="41"/>
       <c r="C170" s="43" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="D170" s="44" t="s">
-        <v>319</v>
+        <v>353</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="41"/>
       <c r="B171" s="41"/>
       <c r="C171" s="43" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="D171" s="44" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="41"/>
       <c r="B172" s="41"/>
       <c r="C172" s="43" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="D172" s="44" t="s">
-        <v>1429</v>
+        <v>317</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17772,44 +17788,44 @@
         <v>1432</v>
       </c>
       <c r="D174" s="44" t="s">
-        <v>979</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="41"/>
       <c r="B175" s="41"/>
       <c r="C175" s="43" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="D175" s="44" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="41"/>
       <c r="B176" s="41"/>
-      <c r="C176" s="45" t="s">
-        <v>1434</v>
-      </c>
-      <c r="D176" s="46" t="s">
+      <c r="C176" s="43" t="s">
         <v>1435</v>
       </c>
-      <c r="E176" s="45"/>
+      <c r="D176" s="44" t="s">
+        <v>980</v>
+      </c>
     </row>
     <row r="177" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="41" t="s">
+      <c r="A177" s="41"/>
+      <c r="B177" s="41"/>
+      <c r="C177" s="45" t="s">
         <v>1436</v>
       </c>
-      <c r="B177" s="41"/>
-      <c r="C177" s="43" t="s">
+      <c r="D177" s="46" t="s">
         <v>1437</v>
       </c>
-      <c r="D177" s="44" t="s">
+      <c r="E177" s="45"/>
+    </row>
+    <row r="178" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="41" t="s">
         <v>1438</v>
       </c>
-    </row>
-    <row r="178" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="41"/>
       <c r="B178" s="41"/>
       <c r="C178" s="43" t="s">
         <v>1439</v>
@@ -17845,27 +17861,27 @@
         <v>1445</v>
       </c>
       <c r="D181" s="44" t="s">
-        <v>200</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="41"/>
       <c r="B182" s="41"/>
       <c r="C182" s="43" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="D182" s="44" t="s">
-        <v>921</v>
+        <v>200</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="41"/>
       <c r="B183" s="41"/>
       <c r="C183" s="43" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="D183" s="44" t="s">
-        <v>1448</v>
+        <v>921</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17875,17 +17891,17 @@
         <v>1449</v>
       </c>
       <c r="D184" s="44" t="s">
-        <v>198</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="41"/>
       <c r="B185" s="41"/>
       <c r="C185" s="43" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="D185" s="44" t="s">
-        <v>1451</v>
+        <v>198</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17895,27 +17911,27 @@
         <v>1452</v>
       </c>
       <c r="D186" s="44" t="s">
-        <v>190</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="41"/>
       <c r="B187" s="41"/>
       <c r="C187" s="43" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="D187" s="44" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="41"/>
       <c r="B188" s="41"/>
       <c r="C188" s="43" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="D188" s="44" t="s">
-        <v>1455</v>
+        <v>212</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17991,39 +18007,46 @@
     <row r="196" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="41"/>
       <c r="B196" s="41"/>
-      <c r="C196" s="45" t="s">
+      <c r="C196" s="43" t="s">
         <v>1470</v>
       </c>
-      <c r="D196" s="46" t="s">
+      <c r="D196" s="44" t="s">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="41"/>
+      <c r="B197" s="41"/>
+      <c r="C197" s="45" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D197" s="46" t="s">
         <v>210</v>
       </c>
-      <c r="E196" s="45"/>
-    </row>
-    <row r="197" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="48" t="s">
-        <v>1393</v>
-      </c>
-      <c r="B197" s="48"/>
-      <c r="C197" s="49" t="s">
-        <v>1471</v>
-      </c>
-      <c r="D197" s="44" t="s">
+      <c r="E197" s="45"/>
+    </row>
+    <row r="198" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="49" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B198" s="49"/>
+      <c r="C198" s="50" t="s">
+        <v>1473</v>
+      </c>
+      <c r="D198" s="44" t="s">
         <v>562</v>
       </c>
-      <c r="E197" s="43" t="s">
-        <v>1472</v>
-      </c>
-    </row>
-    <row r="198" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="48"/>
-      <c r="B198" s="48"/>
-      <c r="C198" s="49"/>
-      <c r="D198" s="44" t="s">
+      <c r="E198" s="43" t="s">
+        <v>1474</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="49"/>
+      <c r="B199" s="49"/>
+      <c r="C199" s="50"/>
+      <c r="D199" s="44" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="199" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D199" s="44"/>
     </row>
     <row r="200" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D200" s="44"/>
@@ -20548,25 +20571,28 @@
     <row r="1040" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1040" s="44"/>
     </row>
+    <row r="1041" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1041" s="44"/>
+    </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A2:A176"/>
+    <mergeCell ref="A2:A177"/>
     <mergeCell ref="B2:B14"/>
-    <mergeCell ref="B15:B29"/>
-    <mergeCell ref="B30:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B58"/>
-    <mergeCell ref="B59:B116"/>
-    <mergeCell ref="D64:D66"/>
-    <mergeCell ref="E64:E66"/>
-    <mergeCell ref="D67:D70"/>
-    <mergeCell ref="E67:E70"/>
-    <mergeCell ref="B117:B176"/>
-    <mergeCell ref="A177:B196"/>
-    <mergeCell ref="A197:B198"/>
-    <mergeCell ref="C197:C198"/>
+    <mergeCell ref="B15:B30"/>
+    <mergeCell ref="B31:B42"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B51:B59"/>
+    <mergeCell ref="B60:B117"/>
+    <mergeCell ref="D65:D67"/>
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="B118:B177"/>
+    <mergeCell ref="A178:B197"/>
+    <mergeCell ref="A198:B199"/>
+    <mergeCell ref="C198:C199"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
update sheet with latest grav accel additions
</commit_message>
<xml_diff>
--- a/Astro Software.xlsx
+++ b/Astro Software.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Software" sheetId="1" state="visible" r:id="rId3"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2847" uniqueCount="1493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2853" uniqueCount="1497">
   <si>
     <t xml:space="preserve">Astrodynamics Software </t>
   </si>
@@ -3946,13 +3946,25 @@
     <t xml:space="preserve">getnormGottN</t>
   </si>
   <si>
+    <t xml:space="preserve">Covers Gottlieb and Lear approaches</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.astro.perturbations.gravity.accel_gott</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.astro.perturbations.gravity.accel_lear</t>
+  </si>
+  <si>
     <t xml:space="preserve">valladopy.astro.perturbations.gravity.accel_gdts</t>
   </si>
   <si>
     <t xml:space="preserve">GravAccelGDTS</t>
   </si>
   <si>
-    <t xml:space="preserve">valladopy.astro.perturbations.gravity.accel_gott</t>
+    <t xml:space="preserve">valladopy.astro.perturbations.gravity.accel_mont</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.astro.perturbations.gravity.accel_pines</t>
   </si>
   <si>
     <t xml:space="preserve">valladopy.astro.perturbations.utils.legpolyn</t>
@@ -3961,7 +3973,7 @@
     <t xml:space="preserve">legpolyn</t>
   </si>
   <si>
-    <t xml:space="preserve">Covers GTDS &amp; Montenbruck approach</t>
+    <t xml:space="preserve">Covers GTDS &amp; Montenbruck approaches</t>
   </si>
   <si>
     <t xml:space="preserve">valladopy.astro.perturbations.utils.trigpoly</t>
@@ -4707,7 +4719,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d\-mmm"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -4849,12 +4861,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val=""/>
-      <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -5189,7 +5195,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5207,10 +5217,6 @@
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -5467,10 +5473,10 @@
   </sheetPr>
   <dimension ref="A1:P349"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="7" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="7" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I235" activeCellId="0" sqref="I235"/>
+      <selection pane="bottomLeft" activeCell="O233" activeCellId="0" sqref="O233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="11.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7556,25 +7562,35 @@
         <v>209</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" s="13" customFormat="true" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B117" s="1"/>
       <c r="C117" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D117" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="E117" s="1"/>
       <c r="F117" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="G117" s="2"/>
+      <c r="H117" s="2"/>
+      <c r="I117" s="2"/>
       <c r="J117" s="2" t="s">
         <v>210</v>
       </c>
       <c r="K117" s="2" t="s">
         <v>211</v>
       </c>
+      <c r="L117" s="2"/>
+      <c r="M117" s="2"/>
+      <c r="N117" s="2"/>
+      <c r="O117" s="2"/>
+      <c r="P117" s="2"/>
     </row>
     <row r="118" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
@@ -7605,24 +7621,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="119" s="13" customFormat="true" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="1"/>
-      <c r="B119" s="1"/>
-      <c r="C119" s="1"/>
-      <c r="D119" s="1"/>
-      <c r="E119" s="1"/>
-      <c r="F119" s="2"/>
-      <c r="G119" s="2"/>
-      <c r="H119" s="2"/>
-      <c r="I119" s="2"/>
-      <c r="J119" s="2"/>
-      <c r="K119" s="2"/>
-      <c r="L119" s="2"/>
-      <c r="M119" s="2"/>
-      <c r="N119" s="2"/>
-      <c r="O119" s="2"/>
-      <c r="P119" s="2"/>
-    </row>
+    <row r="119" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="120" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="12" t="s">
         <v>214</v>
@@ -9823,9 +9822,6 @@
       <c r="B227" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D227" s="9" t="s">
-        <v>3</v>
-      </c>
       <c r="J227" s="2" t="s">
         <v>397</v>
       </c>
@@ -9835,7 +9831,9 @@
     </row>
     <row r="228" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B228" s="9"/>
-      <c r="D228" s="9"/>
+      <c r="D228" s="9" t="s">
+        <v>3</v>
+      </c>
       <c r="F228" s="9" t="s">
         <v>3</v>
       </c>
@@ -9870,9 +9868,7 @@
       <c r="D230" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F230" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="F230" s="15"/>
       <c r="J230" s="2" t="s">
         <v>403</v>
       </c>
@@ -9887,6 +9883,7 @@
       <c r="D231" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="F231" s="15"/>
       <c r="J231" s="2" t="s">
         <v>405</v>
       </c>
@@ -9929,6 +9926,7 @@
       <c r="D234" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="F234" s="15"/>
       <c r="J234" s="2" t="s">
         <v>411</v>
       </c>
@@ -9960,7 +9958,7 @@
       <c r="D236" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F236" s="7" t="s">
+      <c r="F236" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J236" s="2" t="s">
@@ -9977,7 +9975,7 @@
       <c r="D237" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F237" s="7" t="s">
+      <c r="F237" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J237" s="2" t="s">
@@ -9994,7 +9992,7 @@
       <c r="D238" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F238" s="7" t="s">
+      <c r="F238" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J238" s="2" t="s">
@@ -10423,7 +10421,8 @@
         <v>461</v>
       </c>
     </row>
-    <row r="262" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="262" s="13" customFormat="true" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="1"/>
       <c r="B262" s="10" t="s">
         <v>3</v>
       </c>
@@ -10439,6 +10438,8 @@
       <c r="F262" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="G262" s="2"/>
+      <c r="H262" s="2"/>
       <c r="I262" s="2" t="n">
         <v>310</v>
       </c>
@@ -10448,6 +10449,11 @@
       <c r="K262" s="2" t="s">
         <v>463</v>
       </c>
+      <c r="L262" s="2"/>
+      <c r="M262" s="2"/>
+      <c r="N262" s="2"/>
+      <c r="O262" s="2"/>
+      <c r="P262" s="2"/>
     </row>
     <row r="263" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C263" s="1" t="s">
@@ -10472,24 +10478,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="264" s="13" customFormat="true" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="1"/>
-      <c r="B264" s="1"/>
-      <c r="C264" s="1"/>
-      <c r="D264" s="1"/>
-      <c r="E264" s="1"/>
-      <c r="F264" s="2"/>
-      <c r="G264" s="2"/>
-      <c r="H264" s="2"/>
-      <c r="I264" s="2"/>
-      <c r="J264" s="2"/>
-      <c r="K264" s="2"/>
-      <c r="L264" s="2"/>
-      <c r="M264" s="2"/>
-      <c r="N264" s="2"/>
-      <c r="O264" s="2"/>
-      <c r="P264" s="2"/>
-    </row>
+    <row r="264" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="265" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A265" s="12" t="s">
         <v>466</v>
@@ -10627,39 +10616,34 @@
         <v>474</v>
       </c>
     </row>
-    <row r="274" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="274" s="13" customFormat="true" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="1"/>
       <c r="B274" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="C274" s="1"/>
       <c r="D274" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="E274" s="1"/>
       <c r="F274" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="G274" s="2"/>
+      <c r="H274" s="2"/>
+      <c r="I274" s="2"/>
       <c r="J274" s="2" t="s">
         <v>475</v>
       </c>
+      <c r="K274" s="2"/>
+      <c r="L274" s="2"/>
+      <c r="M274" s="2"/>
+      <c r="N274" s="2"/>
+      <c r="O274" s="2"/>
+      <c r="P274" s="2"/>
     </row>
     <row r="275" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="276" s="13" customFormat="true" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="1"/>
-      <c r="B276" s="1"/>
-      <c r="C276" s="1"/>
-      <c r="D276" s="1"/>
-      <c r="E276" s="1"/>
-      <c r="F276" s="2"/>
-      <c r="G276" s="2"/>
-      <c r="H276" s="2"/>
-      <c r="I276" s="2"/>
-      <c r="J276" s="2"/>
-      <c r="K276" s="2"/>
-      <c r="L276" s="2"/>
-      <c r="M276" s="2"/>
-      <c r="N276" s="2"/>
-      <c r="O276" s="2"/>
-      <c r="P276" s="2"/>
-    </row>
+    <row r="276" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="277" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A277" s="12" t="s">
         <v>476</v>
@@ -10997,7 +10981,24 @@
         <v>499</v>
       </c>
     </row>
-    <row r="291" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="291" s="13" customFormat="true" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="1"/>
+      <c r="B291" s="1"/>
+      <c r="C291" s="1"/>
+      <c r="D291" s="1"/>
+      <c r="E291" s="1"/>
+      <c r="F291" s="2"/>
+      <c r="G291" s="2"/>
+      <c r="H291" s="2"/>
+      <c r="I291" s="2"/>
+      <c r="J291" s="2"/>
+      <c r="K291" s="2"/>
+      <c r="L291" s="2"/>
+      <c r="M291" s="2"/>
+      <c r="N291" s="2"/>
+      <c r="O291" s="2"/>
+      <c r="P291" s="2"/>
+    </row>
     <row r="292" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="7" t="s">
         <v>3</v>
@@ -11012,24 +11013,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="293" s="13" customFormat="true" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="1"/>
-      <c r="B293" s="1"/>
-      <c r="C293" s="1"/>
-      <c r="D293" s="1"/>
-      <c r="E293" s="1"/>
-      <c r="F293" s="2"/>
-      <c r="G293" s="2"/>
-      <c r="H293" s="2"/>
-      <c r="I293" s="2"/>
-      <c r="J293" s="2"/>
-      <c r="K293" s="2"/>
-      <c r="L293" s="2"/>
-      <c r="M293" s="2"/>
-      <c r="N293" s="2"/>
-      <c r="O293" s="2"/>
-      <c r="P293" s="2"/>
-    </row>
+    <row r="293" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="294" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A294" s="12" t="s">
         <v>502</v>
@@ -11817,26 +11801,26 @@
         <v>569</v>
       </c>
     </row>
-    <row r="340" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="340" s="13" customFormat="true" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A340" s="1"/>
+      <c r="B340" s="1"/>
+      <c r="C340" s="1"/>
+      <c r="D340" s="1"/>
+      <c r="E340" s="1"/>
+      <c r="F340" s="2"/>
+      <c r="G340" s="2"/>
+      <c r="H340" s="2"/>
+      <c r="I340" s="2"/>
+      <c r="J340" s="2"/>
+      <c r="K340" s="2"/>
+      <c r="L340" s="2"/>
+      <c r="M340" s="2"/>
+      <c r="N340" s="2"/>
+      <c r="O340" s="2"/>
+      <c r="P340" s="2"/>
+    </row>
     <row r="341" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="342" s="13" customFormat="true" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A342" s="1"/>
-      <c r="B342" s="1"/>
-      <c r="C342" s="1"/>
-      <c r="D342" s="1"/>
-      <c r="E342" s="1"/>
-      <c r="F342" s="2"/>
-      <c r="G342" s="2"/>
-      <c r="H342" s="2"/>
-      <c r="I342" s="2"/>
-      <c r="J342" s="2"/>
-      <c r="K342" s="2"/>
-      <c r="L342" s="2"/>
-      <c r="M342" s="2"/>
-      <c r="N342" s="2"/>
-      <c r="O342" s="2"/>
-      <c r="P342" s="2"/>
-    </row>
+    <row r="342" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="343" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A343" s="12" t="s">
         <v>570</v>
@@ -14156,8 +14140,42 @@
     <row r="102" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="103" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="104" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="105" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="106" s="25" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="25"/>
+      <c r="B105" s="25"/>
+      <c r="C105" s="25"/>
+      <c r="D105" s="25"/>
+      <c r="E105" s="25"/>
+      <c r="F105" s="25"/>
+      <c r="G105" s="25"/>
+      <c r="H105" s="25"/>
+      <c r="I105" s="25"/>
+      <c r="J105" s="25"/>
+      <c r="K105" s="25"/>
+      <c r="L105" s="25"/>
+      <c r="M105" s="25"/>
+      <c r="N105" s="25"/>
+      <c r="O105" s="25"/>
+      <c r="P105" s="25"/>
+    </row>
+    <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="25"/>
+      <c r="B106" s="25"/>
+      <c r="C106" s="25"/>
+      <c r="D106" s="25"/>
+      <c r="E106" s="25"/>
+      <c r="F106" s="25"/>
+      <c r="G106" s="25"/>
+      <c r="H106" s="25"/>
+      <c r="I106" s="25"/>
+      <c r="J106" s="25"/>
+      <c r="K106" s="25"/>
+      <c r="L106" s="25"/>
+      <c r="M106" s="25"/>
+      <c r="N106" s="25"/>
+      <c r="O106" s="25"/>
+      <c r="P106" s="25"/>
+    </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="25"/>
       <c r="B107" s="25"/>
@@ -14730,17 +14748,43 @@
         <v>206</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" s="36" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0"/>
       <c r="B67" s="24" t="s">
         <v>208</v>
       </c>
+      <c r="C67" s="0"/>
+      <c r="D67" s="0"/>
+      <c r="E67" s="0"/>
+      <c r="F67" s="0"/>
+      <c r="G67" s="0"/>
+      <c r="H67" s="0"/>
+      <c r="I67" s="0"/>
+      <c r="J67" s="0"/>
+      <c r="K67" s="0"/>
+      <c r="L67" s="0"/>
+      <c r="M67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="24" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="69" s="36" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="36"/>
+      <c r="B69" s="36"/>
+      <c r="C69" s="36"/>
+      <c r="D69" s="36"/>
+      <c r="E69" s="36"/>
+      <c r="F69" s="36"/>
+      <c r="G69" s="36"/>
+      <c r="H69" s="36"/>
+      <c r="I69" s="36"/>
+      <c r="J69" s="36"/>
+      <c r="K69" s="36"/>
+      <c r="L69" s="36"/>
+      <c r="M69" s="36"/>
+    </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="36" t="s">
         <v>894</v>
@@ -15609,7 +15653,36 @@
         <v>454</v>
       </c>
     </row>
-    <row r="223" s="36" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="221" s="36" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="0"/>
+      <c r="B221" s="0"/>
+      <c r="C221" s="0"/>
+      <c r="D221" s="0"/>
+      <c r="E221" s="0"/>
+      <c r="F221" s="0"/>
+      <c r="G221" s="0"/>
+      <c r="H221" s="0"/>
+      <c r="I221" s="0"/>
+      <c r="J221" s="0"/>
+      <c r="K221" s="0"/>
+      <c r="L221" s="0"/>
+      <c r="M221" s="0"/>
+    </row>
+    <row r="223" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="36"/>
+      <c r="B223" s="36"/>
+      <c r="C223" s="36"/>
+      <c r="D223" s="36"/>
+      <c r="E223" s="36"/>
+      <c r="F223" s="36"/>
+      <c r="G223" s="36"/>
+      <c r="H223" s="36"/>
+      <c r="I223" s="36"/>
+      <c r="J223" s="36"/>
+      <c r="K223" s="36"/>
+      <c r="L223" s="36"/>
+      <c r="M223" s="36"/>
+    </row>
     <row r="224" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="36" t="s">
         <v>894</v>
@@ -15789,12 +15862,38 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="257" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="257" s="36" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="24" t="s">
         <v>1061</v>
       </c>
-    </row>
-    <row r="259" s="36" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B257" s="0"/>
+      <c r="C257" s="0"/>
+      <c r="D257" s="0"/>
+      <c r="E257" s="0"/>
+      <c r="F257" s="0"/>
+      <c r="G257" s="0"/>
+      <c r="H257" s="0"/>
+      <c r="I257" s="0"/>
+      <c r="J257" s="0"/>
+      <c r="K257" s="0"/>
+      <c r="L257" s="0"/>
+      <c r="M257" s="0"/>
+    </row>
+    <row r="259" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="36"/>
+      <c r="B259" s="36"/>
+      <c r="C259" s="36"/>
+      <c r="D259" s="36"/>
+      <c r="E259" s="36"/>
+      <c r="F259" s="36"/>
+      <c r="G259" s="36"/>
+      <c r="H259" s="36"/>
+      <c r="I259" s="36"/>
+      <c r="J259" s="36"/>
+      <c r="K259" s="36"/>
+      <c r="L259" s="36"/>
+      <c r="M259" s="36"/>
+    </row>
     <row r="260" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="36" t="s">
         <v>894</v>
@@ -16235,10 +16334,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB1046"/>
+  <dimension ref="A1:AB1049"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D41" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E53" activeCellId="0" sqref="E53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D56" activeCellId="0" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16813,31 +16912,33 @@
       <c r="D50" s="44" t="s">
         <v>1241</v>
       </c>
-      <c r="E50" s="43"/>
+      <c r="E50" s="43" t="s">
+        <v>1242</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="41"/>
       <c r="B51" s="41"/>
       <c r="C51" s="43" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="D51" s="44" t="s">
-        <v>1243</v>
+        <v>421</v>
       </c>
       <c r="E51" s="43"/>
     </row>
     <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="41"/>
       <c r="B52" s="41"/>
-      <c r="C52" s="43" t="s">
+      <c r="C52" s="49" t="s">
         <v>1244</v>
       </c>
       <c r="D52" s="44" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="E52" s="43"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="41"/>
       <c r="B53" s="41"/>
       <c r="C53" s="43" t="s">
@@ -16846,88 +16947,82 @@
       <c r="D53" s="44" t="s">
         <v>1246</v>
       </c>
-      <c r="E53" s="49" t="s">
-        <v>1247</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E53" s="43"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="41"/>
       <c r="B54" s="41"/>
-      <c r="C54" s="45" t="s">
-        <v>1248</v>
-      </c>
-      <c r="D54" s="46" t="s">
-        <v>1249</v>
-      </c>
-      <c r="E54" s="50" t="s">
+      <c r="C54" s="43" t="s">
         <v>1247</v>
       </c>
+      <c r="D54" s="44" t="s">
+        <v>415</v>
+      </c>
+      <c r="E54" s="43"/>
     </row>
     <row r="55" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="41"/>
-      <c r="B55" s="41" t="s">
-        <v>1250</v>
-      </c>
+      <c r="B55" s="41"/>
       <c r="C55" s="43" t="s">
-        <v>1251</v>
+        <v>1248</v>
       </c>
       <c r="D55" s="44" t="s">
-        <v>486</v>
-      </c>
-      <c r="E55" s="43" t="s">
-        <v>1252</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>419</v>
+      </c>
+      <c r="E55" s="43"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="41"/>
       <c r="B56" s="41"/>
       <c r="C56" s="43" t="s">
-        <v>1253</v>
+        <v>1249</v>
       </c>
       <c r="D56" s="44" t="s">
-        <v>484</v>
-      </c>
-      <c r="E56" s="43" t="s">
-        <v>1252</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1250</v>
+      </c>
+      <c r="E56" s="50" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="41"/>
       <c r="B57" s="41"/>
-      <c r="C57" s="43" t="s">
-        <v>1254</v>
-      </c>
-      <c r="D57" s="44" t="s">
-        <v>480</v>
-      </c>
-      <c r="E57" s="43" t="s">
+      <c r="C57" s="45" t="s">
         <v>1252</v>
+      </c>
+      <c r="D57" s="46" t="s">
+        <v>1253</v>
+      </c>
+      <c r="E57" s="51" t="s">
+        <v>1251</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="41"/>
-      <c r="B58" s="41"/>
+      <c r="B58" s="41" t="s">
+        <v>1254</v>
+      </c>
       <c r="C58" s="43" t="s">
         <v>1255</v>
       </c>
       <c r="D58" s="44" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="E58" s="43" t="s">
-        <v>1252</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="41"/>
       <c r="B59" s="41"/>
       <c r="C59" s="43" t="s">
+        <v>1257</v>
+      </c>
+      <c r="D59" s="44" t="s">
+        <v>484</v>
+      </c>
+      <c r="E59" s="43" t="s">
         <v>1256</v>
-      </c>
-      <c r="D59" s="44" t="s">
-        <v>495</v>
-      </c>
-      <c r="E59" s="43" t="s">
-        <v>1257</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16937,10 +17032,10 @@
         <v>1258</v>
       </c>
       <c r="D60" s="44" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="E60" s="43" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16950,10 +17045,10 @@
         <v>1259</v>
       </c>
       <c r="D61" s="44" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="E61" s="43" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16963,33 +17058,36 @@
         <v>1260</v>
       </c>
       <c r="D62" s="44" t="s">
-        <v>1250</v>
+        <v>495</v>
       </c>
       <c r="E62" s="43" t="s">
-        <v>1257</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="41"/>
       <c r="B63" s="41"/>
-      <c r="C63" s="45" t="s">
+      <c r="C63" s="43" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D63" s="44" t="s">
+        <v>478</v>
+      </c>
+      <c r="E63" s="43" t="s">
         <v>1261</v>
       </c>
-      <c r="D63" s="46" t="s">
-        <v>492</v>
-      </c>
-      <c r="E63" s="45"/>
     </row>
     <row r="64" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="41"/>
-      <c r="B64" s="41" t="s">
-        <v>1262</v>
-      </c>
+      <c r="B64" s="41"/>
       <c r="C64" s="43" t="s">
         <v>1263</v>
       </c>
       <c r="D64" s="44" t="s">
-        <v>468</v>
+        <v>488</v>
+      </c>
+      <c r="E64" s="43" t="s">
+        <v>1261</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16999,81 +17097,86 @@
         <v>1264</v>
       </c>
       <c r="D65" s="44" t="s">
-        <v>469</v>
+        <v>1254</v>
+      </c>
+      <c r="E65" s="43" t="s">
+        <v>1261</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="41"/>
       <c r="B66" s="41"/>
-      <c r="C66" s="43" t="s">
+      <c r="C66" s="45" t="s">
         <v>1265</v>
       </c>
-      <c r="D66" s="44" t="s">
-        <v>232</v>
-      </c>
+      <c r="D66" s="46" t="s">
+        <v>492</v>
+      </c>
+      <c r="E66" s="45"/>
     </row>
     <row r="67" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="41"/>
-      <c r="B67" s="41"/>
+      <c r="B67" s="41" t="s">
+        <v>1266</v>
+      </c>
       <c r="C67" s="43" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="D67" s="44" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="41"/>
       <c r="B68" s="41"/>
       <c r="C68" s="43" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="D68" s="44" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="41"/>
       <c r="B69" s="41"/>
       <c r="C69" s="43" t="s">
-        <v>1268</v>
-      </c>
-      <c r="D69" s="51" t="s">
         <v>1269</v>
       </c>
-      <c r="E69" s="52" t="s">
-        <v>1270</v>
+      <c r="D69" s="44" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="41"/>
       <c r="B70" s="41"/>
       <c r="C70" s="43" t="s">
-        <v>1271</v>
-      </c>
-      <c r="D70" s="51"/>
-      <c r="E70" s="51"/>
+        <v>1270</v>
+      </c>
+      <c r="D70" s="44" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="41"/>
       <c r="B71" s="41"/>
       <c r="C71" s="43" t="s">
-        <v>1272</v>
-      </c>
-      <c r="D71" s="51"/>
-      <c r="E71" s="51"/>
+        <v>1271</v>
+      </c>
+      <c r="D71" s="44" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="41"/>
       <c r="B72" s="41"/>
       <c r="C72" s="43" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D72" s="52" t="s">
         <v>1273</v>
       </c>
-      <c r="D72" s="51" t="s">
+      <c r="E72" s="53" t="s">
         <v>1274</v>
-      </c>
-      <c r="E72" s="52" t="s">
-        <v>1270</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17082,8 +17185,8 @@
       <c r="C73" s="43" t="s">
         <v>1275</v>
       </c>
-      <c r="D73" s="51"/>
-      <c r="E73" s="51"/>
+      <c r="D73" s="52"/>
+      <c r="E73" s="52"/>
     </row>
     <row r="74" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="41"/>
@@ -17091,8 +17194,8 @@
       <c r="C74" s="43" t="s">
         <v>1276</v>
       </c>
-      <c r="D74" s="51"/>
-      <c r="E74" s="51"/>
+      <c r="D74" s="52"/>
+      <c r="E74" s="52"/>
     </row>
     <row r="75" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="41"/>
@@ -17100,18 +17203,21 @@
       <c r="C75" s="43" t="s">
         <v>1277</v>
       </c>
-      <c r="D75" s="51"/>
-      <c r="E75" s="51"/>
+      <c r="D75" s="52" t="s">
+        <v>1278</v>
+      </c>
+      <c r="E75" s="53" t="s">
+        <v>1274</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="41"/>
       <c r="B76" s="41"/>
       <c r="C76" s="43" t="s">
-        <v>1278</v>
-      </c>
-      <c r="D76" s="44" t="s">
         <v>1279</v>
       </c>
+      <c r="D76" s="52"/>
+      <c r="E76" s="52"/>
     </row>
     <row r="77" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="41"/>
@@ -17119,328 +17225,326 @@
       <c r="C77" s="43" t="s">
         <v>1280</v>
       </c>
-      <c r="D77" s="44" t="s">
-        <v>1281</v>
-      </c>
+      <c r="D77" s="52"/>
+      <c r="E77" s="52"/>
     </row>
     <row r="78" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="41"/>
       <c r="B78" s="41"/>
       <c r="C78" s="43" t="s">
-        <v>1282</v>
-      </c>
-      <c r="D78" s="44" t="s">
-        <v>1283</v>
-      </c>
+        <v>1281</v>
+      </c>
+      <c r="D78" s="52"/>
+      <c r="E78" s="52"/>
     </row>
     <row r="79" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="41"/>
       <c r="B79" s="41"/>
       <c r="C79" s="43" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="D79" s="44" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="41"/>
       <c r="B80" s="41"/>
       <c r="C80" s="43" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="D80" s="44" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="41"/>
       <c r="B81" s="41"/>
       <c r="C81" s="43" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="D81" s="44" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="41"/>
       <c r="B82" s="41"/>
       <c r="C82" s="43" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="D82" s="44" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="41"/>
       <c r="B83" s="41"/>
       <c r="C83" s="43" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="D83" s="44" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="41"/>
       <c r="B84" s="41"/>
       <c r="C84" s="43" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="D84" s="44" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="41"/>
       <c r="B85" s="41"/>
       <c r="C85" s="43" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="D85" s="44" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="41"/>
       <c r="B86" s="41"/>
       <c r="C86" s="43" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="D86" s="44" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="41"/>
       <c r="B87" s="41"/>
       <c r="C87" s="43" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="D87" s="44" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="41"/>
       <c r="B88" s="41"/>
       <c r="C88" s="43" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="D88" s="44" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="41"/>
       <c r="B89" s="41"/>
       <c r="C89" s="43" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="D89" s="44" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="41"/>
       <c r="B90" s="41"/>
       <c r="C90" s="43" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="D90" s="44" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="41"/>
       <c r="B91" s="41"/>
       <c r="C91" s="43" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="D91" s="44" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="41"/>
       <c r="B92" s="41"/>
       <c r="C92" s="43" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="D92" s="44" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="41"/>
       <c r="B93" s="41"/>
       <c r="C93" s="43" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="D93" s="44" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="41"/>
       <c r="B94" s="41"/>
       <c r="C94" s="43" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="D94" s="44" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="41"/>
       <c r="B95" s="41"/>
       <c r="C95" s="43" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="D95" s="44" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="41"/>
       <c r="B96" s="41"/>
       <c r="C96" s="43" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="D96" s="44" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="41"/>
       <c r="B97" s="41"/>
       <c r="C97" s="43" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="D97" s="44" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="41"/>
       <c r="B98" s="41"/>
       <c r="C98" s="43" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="D98" s="44" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="41"/>
       <c r="B99" s="41"/>
       <c r="C99" s="43" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="D99" s="44" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="41"/>
       <c r="B100" s="41"/>
       <c r="C100" s="43" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="D100" s="44" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="41"/>
       <c r="B101" s="41"/>
       <c r="C101" s="43" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="D101" s="44" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="41"/>
       <c r="B102" s="41"/>
       <c r="C102" s="43" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="D102" s="44" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="41"/>
       <c r="B103" s="41"/>
       <c r="C103" s="43" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D103" s="44" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="41"/>
       <c r="B104" s="41"/>
       <c r="C104" s="43" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D104" s="44" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="41"/>
       <c r="B105" s="41"/>
       <c r="C105" s="43" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="D105" s="44" t="s">
-        <v>219</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="41"/>
       <c r="B106" s="41"/>
       <c r="C106" s="43" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D106" s="44" t="s">
         <v>1337</v>
-      </c>
-      <c r="D106" s="44" t="s">
-        <v>1338</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="41"/>
       <c r="B107" s="41"/>
       <c r="C107" s="43" t="s">
+        <v>1338</v>
+      </c>
+      <c r="D107" s="44" t="s">
         <v>1339</v>
-      </c>
-      <c r="D107" s="44" t="s">
-        <v>1340</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="41"/>
       <c r="B108" s="41"/>
       <c r="C108" s="43" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="D108" s="44" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="41"/>
       <c r="B109" s="41"/>
       <c r="C109" s="43" t="s">
+        <v>1341</v>
+      </c>
+      <c r="D109" s="44" t="s">
         <v>1342</v>
-      </c>
-      <c r="D109" s="44" t="s">
-        <v>972</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17450,47 +17554,47 @@
         <v>1343</v>
       </c>
       <c r="D110" s="44" t="s">
-        <v>227</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="41"/>
       <c r="B111" s="41"/>
       <c r="C111" s="43" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="D111" s="44" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="41"/>
       <c r="B112" s="41"/>
       <c r="C112" s="43" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="D112" s="44" t="s">
-        <v>471</v>
+        <v>972</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="41"/>
       <c r="B113" s="41"/>
       <c r="C113" s="43" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="D113" s="44" t="s">
-        <v>971</v>
+        <v>227</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="41"/>
       <c r="B114" s="41"/>
       <c r="C114" s="43" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="D114" s="44" t="s">
-        <v>1348</v>
+        <v>229</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17500,7 +17604,7 @@
         <v>1349</v>
       </c>
       <c r="D115" s="44" t="s">
-        <v>223</v>
+        <v>471</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17510,7 +17614,7 @@
         <v>1350</v>
       </c>
       <c r="D116" s="44" t="s">
-        <v>241</v>
+        <v>971</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17520,122 +17624,119 @@
         <v>1351</v>
       </c>
       <c r="D117" s="44" t="s">
-        <v>225</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="41"/>
       <c r="B118" s="41"/>
       <c r="C118" s="43" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="D118" s="44" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="41"/>
       <c r="B119" s="41"/>
       <c r="C119" s="43" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="D119" s="44" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="41"/>
       <c r="B120" s="41"/>
       <c r="C120" s="43" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="D120" s="44" t="s">
-        <v>475</v>
-      </c>
-      <c r="E120" s="43" t="s">
-        <v>1355</v>
+        <v>225</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="41"/>
       <c r="B121" s="41"/>
-      <c r="C121" s="45" t="s">
+      <c r="C121" s="43" t="s">
         <v>1356</v>
       </c>
-      <c r="D121" s="46" t="s">
-        <v>474</v>
-      </c>
-      <c r="E121" s="45"/>
+      <c r="D121" s="44" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="122" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="41"/>
-      <c r="B122" s="41" t="s">
+      <c r="B122" s="41"/>
+      <c r="C122" s="43" t="s">
         <v>1357</v>
       </c>
-      <c r="C122" s="43" t="s">
-        <v>1358</v>
-      </c>
       <c r="D122" s="44" t="s">
-        <v>1359</v>
-      </c>
-      <c r="E122" s="43" t="s">
-        <v>1360</v>
+        <v>239</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="41"/>
       <c r="B123" s="41"/>
       <c r="C123" s="43" t="s">
-        <v>1361</v>
+        <v>1358</v>
       </c>
       <c r="D123" s="44" t="s">
-        <v>1362</v>
+        <v>475</v>
       </c>
       <c r="E123" s="43" t="s">
-        <v>1363</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="41"/>
       <c r="B124" s="41"/>
-      <c r="C124" s="43" t="s">
-        <v>1364</v>
-      </c>
-      <c r="D124" s="44" t="s">
-        <v>438</v>
-      </c>
-      <c r="E124" s="43"/>
+      <c r="C124" s="45" t="s">
+        <v>1360</v>
+      </c>
+      <c r="D124" s="46" t="s">
+        <v>474</v>
+      </c>
+      <c r="E124" s="45"/>
     </row>
     <row r="125" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="41"/>
-      <c r="B125" s="41"/>
+      <c r="B125" s="41" t="s">
+        <v>1361</v>
+      </c>
       <c r="C125" s="43" t="s">
-        <v>1365</v>
+        <v>1362</v>
       </c>
       <c r="D125" s="44" t="s">
-        <v>440</v>
-      </c>
-      <c r="E125" s="43"/>
+        <v>1363</v>
+      </c>
+      <c r="E125" s="43" t="s">
+        <v>1364</v>
+      </c>
     </row>
     <row r="126" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="41"/>
       <c r="B126" s="41"/>
       <c r="C126" s="43" t="s">
+        <v>1365</v>
+      </c>
+      <c r="D126" s="44" t="s">
         <v>1366</v>
       </c>
-      <c r="D126" s="44" t="s">
-        <v>442</v>
-      </c>
-      <c r="E126" s="43"/>
+      <c r="E126" s="43" t="s">
+        <v>1367</v>
+      </c>
     </row>
     <row r="127" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="41"/>
       <c r="B127" s="41"/>
       <c r="C127" s="43" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="D127" s="44" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="E127" s="43"/>
     </row>
@@ -17643,10 +17744,10 @@
       <c r="A128" s="41"/>
       <c r="B128" s="41"/>
       <c r="C128" s="43" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="D128" s="44" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="E128" s="43"/>
     </row>
@@ -17654,10 +17755,10 @@
       <c r="A129" s="41"/>
       <c r="B129" s="41"/>
       <c r="C129" s="43" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="D129" s="44" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="E129" s="43"/>
     </row>
@@ -17665,10 +17766,10 @@
       <c r="A130" s="41"/>
       <c r="B130" s="41"/>
       <c r="C130" s="43" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="D130" s="44" t="s">
-        <v>1371</v>
+        <v>444</v>
       </c>
       <c r="E130" s="43"/>
     </row>
@@ -17679,7 +17780,7 @@
         <v>1372</v>
       </c>
       <c r="D131" s="44" t="s">
-        <v>1373</v>
+        <v>446</v>
       </c>
       <c r="E131" s="43"/>
     </row>
@@ -17687,10 +17788,10 @@
       <c r="A132" s="41"/>
       <c r="B132" s="41"/>
       <c r="C132" s="43" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="D132" s="44" t="s">
-        <v>430</v>
+        <v>448</v>
       </c>
       <c r="E132" s="43"/>
     </row>
@@ -17698,10 +17799,10 @@
       <c r="A133" s="41"/>
       <c r="B133" s="41"/>
       <c r="C133" s="43" t="s">
+        <v>1374</v>
+      </c>
+      <c r="D133" s="44" t="s">
         <v>1375</v>
-      </c>
-      <c r="D133" s="44" t="s">
-        <v>428</v>
       </c>
       <c r="E133" s="43"/>
     </row>
@@ -17714,78 +17815,81 @@
       <c r="D134" s="44" t="s">
         <v>1377</v>
       </c>
-      <c r="E134" s="43" t="s">
-        <v>1378</v>
-      </c>
+      <c r="E134" s="43"/>
     </row>
     <row r="135" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="41"/>
       <c r="B135" s="41"/>
       <c r="C135" s="43" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="D135" s="44" t="s">
-        <v>287</v>
-      </c>
+        <v>430</v>
+      </c>
+      <c r="E135" s="43"/>
     </row>
     <row r="136" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="41"/>
       <c r="B136" s="41"/>
       <c r="C136" s="43" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="D136" s="44" t="s">
-        <v>285</v>
-      </c>
+        <v>428</v>
+      </c>
+      <c r="E136" s="43"/>
     </row>
     <row r="137" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="41"/>
       <c r="B137" s="41"/>
       <c r="C137" s="43" t="s">
+        <v>1380</v>
+      </c>
+      <c r="D137" s="44" t="s">
         <v>1381</v>
       </c>
-      <c r="D137" s="44" t="s">
-        <v>275</v>
+      <c r="E137" s="43" t="s">
+        <v>1382</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="41"/>
       <c r="B138" s="41"/>
       <c r="C138" s="43" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="D138" s="44" t="s">
-        <v>273</v>
+        <v>287</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="41"/>
       <c r="B139" s="41"/>
       <c r="C139" s="43" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="D139" s="44" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="41"/>
       <c r="B140" s="41"/>
       <c r="C140" s="43" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="D140" s="44" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="41"/>
       <c r="B141" s="41"/>
       <c r="C141" s="43" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="D141" s="44" t="s">
-        <v>1386</v>
+        <v>273</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17795,39 +17899,39 @@
         <v>1387</v>
       </c>
       <c r="D142" s="44" t="s">
-        <v>1388</v>
-      </c>
-      <c r="E142" s="43" t="s">
-        <v>1389</v>
+        <v>279</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="41"/>
       <c r="B143" s="41"/>
       <c r="C143" s="43" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="D143" s="44" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="41"/>
       <c r="B144" s="41"/>
       <c r="C144" s="43" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="D144" s="44" t="s">
-        <v>281</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="41"/>
       <c r="B145" s="41"/>
       <c r="C145" s="43" t="s">
+        <v>1391</v>
+      </c>
+      <c r="D145" s="44" t="s">
         <v>1392</v>
       </c>
-      <c r="D145" s="44" t="s">
+      <c r="E145" s="43" t="s">
         <v>1393</v>
       </c>
     </row>
@@ -17838,136 +17942,136 @@
         <v>1394</v>
       </c>
       <c r="D146" s="44" t="s">
-        <v>1395</v>
+        <v>283</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="41"/>
       <c r="B147" s="41"/>
       <c r="C147" s="43" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="D147" s="44" t="s">
-        <v>1397</v>
+        <v>281</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="41"/>
       <c r="B148" s="41"/>
       <c r="C148" s="43" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
       <c r="D148" s="44" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="41"/>
       <c r="B149" s="41"/>
       <c r="C149" s="43" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
       <c r="D149" s="44" t="s">
-        <v>1401</v>
-      </c>
-      <c r="E149" s="53" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="41"/>
       <c r="B150" s="41"/>
       <c r="C150" s="43" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
       <c r="D150" s="44" t="s">
-        <v>1404</v>
-      </c>
-      <c r="E150" s="53" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="41"/>
       <c r="B151" s="41"/>
       <c r="C151" s="43" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
       <c r="D151" s="44" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="41"/>
       <c r="B152" s="41"/>
       <c r="C152" s="43" t="s">
-        <v>1407</v>
+        <v>1404</v>
       </c>
       <c r="D152" s="44" t="s">
-        <v>1408</v>
+        <v>1405</v>
+      </c>
+      <c r="E152" s="50" t="s">
+        <v>1406</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="41"/>
       <c r="B153" s="41"/>
       <c r="C153" s="43" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="D153" s="44" t="s">
-        <v>1410</v>
+        <v>1408</v>
+      </c>
+      <c r="E153" s="50" t="s">
+        <v>1406</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="41"/>
       <c r="B154" s="41"/>
       <c r="C154" s="43" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="D154" s="44" t="s">
-        <v>1412</v>
-      </c>
-      <c r="E154" s="53" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="41"/>
       <c r="B155" s="41"/>
       <c r="C155" s="43" t="s">
-        <v>1414</v>
+        <v>1411</v>
       </c>
       <c r="D155" s="44" t="s">
-        <v>305</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="41"/>
       <c r="B156" s="41"/>
       <c r="C156" s="43" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
       <c r="D156" s="44" t="s">
-        <v>307</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="41"/>
       <c r="B157" s="41"/>
       <c r="C157" s="43" t="s">
+        <v>1415</v>
+      </c>
+      <c r="D157" s="44" t="s">
         <v>1416</v>
       </c>
-      <c r="D157" s="44" t="s">
-        <v>309</v>
+      <c r="E157" s="50" t="s">
+        <v>1417</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="41"/>
       <c r="B158" s="41"/>
       <c r="C158" s="43" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="D158" s="44" t="s">
-        <v>1418</v>
+        <v>305</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17977,73 +18081,73 @@
         <v>1419</v>
       </c>
       <c r="D159" s="44" t="s">
-        <v>1420</v>
+        <v>307</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="41"/>
       <c r="B160" s="41"/>
       <c r="C160" s="43" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D160" s="44" t="s">
-        <v>1422</v>
-      </c>
-      <c r="E160" s="43" t="s">
-        <v>1423</v>
+        <v>309</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="41"/>
       <c r="B161" s="41"/>
       <c r="C161" s="43" t="s">
-        <v>1424</v>
+        <v>1421</v>
       </c>
       <c r="D161" s="44" t="s">
-        <v>1425</v>
-      </c>
-      <c r="E161" s="43" t="s">
-        <v>1426</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="41"/>
       <c r="B162" s="41"/>
       <c r="C162" s="43" t="s">
-        <v>1427</v>
+        <v>1423</v>
       </c>
       <c r="D162" s="44" t="s">
-        <v>995</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="41"/>
       <c r="B163" s="41"/>
       <c r="C163" s="43" t="s">
-        <v>1428</v>
+        <v>1425</v>
       </c>
       <c r="D163" s="44" t="s">
-        <v>996</v>
+        <v>1426</v>
+      </c>
+      <c r="E163" s="43" t="s">
+        <v>1427</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="41"/>
       <c r="B164" s="41"/>
       <c r="C164" s="43" t="s">
+        <v>1428</v>
+      </c>
+      <c r="D164" s="44" t="s">
         <v>1429</v>
       </c>
-      <c r="D164" s="44" t="s">
-        <v>324</v>
+      <c r="E164" s="43" t="s">
+        <v>1430</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="41"/>
       <c r="B165" s="41"/>
       <c r="C165" s="43" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="D165" s="44" t="s">
-        <v>1431</v>
+        <v>995</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18053,27 +18157,27 @@
         <v>1432</v>
       </c>
       <c r="D166" s="44" t="s">
-        <v>1433</v>
+        <v>996</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="41"/>
       <c r="B167" s="41"/>
       <c r="C167" s="43" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="D167" s="44" t="s">
-        <v>988</v>
+        <v>324</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="41"/>
       <c r="B168" s="41"/>
       <c r="C168" s="43" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D168" s="44" t="s">
         <v>1435</v>
-      </c>
-      <c r="D168" s="44" t="s">
-        <v>984</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18083,27 +18187,27 @@
         <v>1436</v>
       </c>
       <c r="D169" s="44" t="s">
-        <v>987</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="41"/>
       <c r="B170" s="41"/>
       <c r="C170" s="43" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="D170" s="44" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="41"/>
       <c r="B171" s="41"/>
       <c r="C171" s="43" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="D171" s="44" t="s">
-        <v>1439</v>
+        <v>984</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18113,37 +18217,37 @@
         <v>1440</v>
       </c>
       <c r="D172" s="44" t="s">
-        <v>1441</v>
+        <v>987</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="41"/>
       <c r="B173" s="41"/>
       <c r="C173" s="43" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="D173" s="44" t="s">
-        <v>1443</v>
+        <v>986</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="41"/>
       <c r="B174" s="41"/>
       <c r="C174" s="43" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="D174" s="44" t="s">
-        <v>353</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="41"/>
       <c r="B175" s="41"/>
       <c r="C175" s="43" t="s">
+        <v>1444</v>
+      </c>
+      <c r="D175" s="44" t="s">
         <v>1445</v>
-      </c>
-      <c r="D175" s="44" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18153,17 +18257,17 @@
         <v>1446</v>
       </c>
       <c r="D176" s="44" t="s">
-        <v>317</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="41"/>
       <c r="B177" s="41"/>
       <c r="C177" s="43" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="D177" s="44" t="s">
-        <v>1448</v>
+        <v>353</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18173,27 +18277,27 @@
         <v>1449</v>
       </c>
       <c r="D178" s="44" t="s">
-        <v>1450</v>
+        <v>319</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="41"/>
       <c r="B179" s="41"/>
       <c r="C179" s="43" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="D179" s="44" t="s">
-        <v>989</v>
+        <v>317</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="41"/>
       <c r="B180" s="41"/>
       <c r="C180" s="43" t="s">
+        <v>1451</v>
+      </c>
+      <c r="D180" s="44" t="s">
         <v>1452</v>
-      </c>
-      <c r="D180" s="44" t="s">
-        <v>990</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18203,80 +18307,80 @@
         <v>1453</v>
       </c>
       <c r="D181" s="44" t="s">
-        <v>991</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="41"/>
       <c r="B182" s="41"/>
-      <c r="C182" s="45" t="s">
-        <v>1454</v>
-      </c>
-      <c r="D182" s="46" t="s">
+      <c r="C182" s="43" t="s">
         <v>1455</v>
       </c>
-      <c r="E182" s="45"/>
+      <c r="D182" s="44" t="s">
+        <v>989</v>
+      </c>
     </row>
     <row r="183" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="41" t="s">
-        <v>1456</v>
-      </c>
+      <c r="A183" s="41"/>
       <c r="B183" s="41"/>
       <c r="C183" s="43" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="D183" s="44" t="s">
-        <v>1458</v>
+        <v>990</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="41"/>
       <c r="B184" s="41"/>
       <c r="C184" s="43" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="D184" s="44" t="s">
-        <v>1460</v>
+        <v>991</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="41"/>
       <c r="B185" s="41"/>
-      <c r="C185" s="43" t="s">
-        <v>1461</v>
-      </c>
-      <c r="D185" s="44" t="s">
-        <v>1462</v>
-      </c>
+      <c r="C185" s="45" t="s">
+        <v>1458</v>
+      </c>
+      <c r="D185" s="46" t="s">
+        <v>1459</v>
+      </c>
+      <c r="E185" s="45"/>
     </row>
     <row r="186" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="41"/>
+      <c r="A186" s="41" t="s">
+        <v>1460</v>
+      </c>
       <c r="B186" s="41"/>
       <c r="C186" s="43" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="D186" s="44" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="41"/>
       <c r="B187" s="41"/>
       <c r="C187" s="43" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
       <c r="D187" s="44" t="s">
-        <v>200</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="41"/>
       <c r="B188" s="41"/>
       <c r="C188" s="43" t="s">
+        <v>1465</v>
+      </c>
+      <c r="D188" s="44" t="s">
         <v>1466</v>
-      </c>
-      <c r="D188" s="44" t="s">
-        <v>931</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18296,7 +18400,7 @@
         <v>1469</v>
       </c>
       <c r="D190" s="44" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18306,17 +18410,17 @@
         <v>1470</v>
       </c>
       <c r="D191" s="44" t="s">
-        <v>1471</v>
+        <v>931</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="41"/>
       <c r="B192" s="41"/>
       <c r="C192" s="43" t="s">
+        <v>1471</v>
+      </c>
+      <c r="D192" s="44" t="s">
         <v>1472</v>
-      </c>
-      <c r="D192" s="44" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18326,7 +18430,7 @@
         <v>1473</v>
       </c>
       <c r="D193" s="44" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18346,111 +18450,132 @@
         <v>1476</v>
       </c>
       <c r="D195" s="44" t="s">
-        <v>1477</v>
+        <v>190</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="41"/>
       <c r="B196" s="41"/>
       <c r="C196" s="43" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="D196" s="44" t="s">
-        <v>1479</v>
+        <v>212</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="41"/>
       <c r="B197" s="41"/>
       <c r="C197" s="43" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="D197" s="44" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="41"/>
       <c r="B198" s="41"/>
       <c r="C198" s="43" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
       <c r="D198" s="44" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="41"/>
       <c r="B199" s="41"/>
       <c r="C199" s="43" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="D199" s="44" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="41"/>
       <c r="B200" s="41"/>
       <c r="C200" s="43" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
       <c r="D200" s="44" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="41"/>
       <c r="B201" s="41"/>
       <c r="C201" s="43" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="D201" s="44" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="41"/>
       <c r="B202" s="41"/>
-      <c r="C202" s="45" t="s">
+      <c r="C202" s="43" t="s">
+        <v>1488</v>
+      </c>
+      <c r="D202" s="44" t="s">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="41"/>
+      <c r="B203" s="41"/>
+      <c r="C203" s="43" t="s">
         <v>1490</v>
       </c>
-      <c r="D202" s="46" t="s">
+      <c r="D203" s="44" t="s">
+        <v>1491</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="41"/>
+      <c r="B204" s="41"/>
+      <c r="C204" s="43" t="s">
+        <v>1492</v>
+      </c>
+      <c r="D204" s="44" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="41"/>
+      <c r="B205" s="41"/>
+      <c r="C205" s="45" t="s">
+        <v>1494</v>
+      </c>
+      <c r="D205" s="46" t="s">
         <v>210</v>
       </c>
-      <c r="E202" s="45"/>
-    </row>
-    <row r="203" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="51" t="s">
-        <v>1412</v>
-      </c>
-      <c r="B203" s="51"/>
-      <c r="C203" s="52" t="s">
-        <v>1491</v>
-      </c>
-      <c r="D203" s="44" t="s">
+      <c r="E205" s="45"/>
+    </row>
+    <row r="206" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="52" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B206" s="52"/>
+      <c r="C206" s="53" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D206" s="44" t="s">
         <v>572</v>
       </c>
-      <c r="E203" s="43" t="s">
-        <v>1492</v>
-      </c>
-    </row>
-    <row r="204" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="51"/>
-      <c r="B204" s="51"/>
-      <c r="C204" s="52"/>
-      <c r="D204" s="44" t="s">
+      <c r="E206" s="43" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="52"/>
+      <c r="B207" s="52"/>
+      <c r="C207" s="53"/>
+      <c r="D207" s="44" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="205" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D205" s="44"/>
-    </row>
-    <row r="206" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D206" s="44"/>
-    </row>
-    <row r="207" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D207" s="44"/>
     </row>
     <row r="208" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D208" s="44"/>
@@ -20969,25 +21094,34 @@
     <row r="1046" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1046" s="44"/>
     </row>
+    <row r="1047" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1047" s="44"/>
+    </row>
+    <row r="1048" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1048" s="44"/>
+    </row>
+    <row r="1049" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1049" s="44"/>
+    </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A2:A182"/>
+    <mergeCell ref="A2:A185"/>
     <mergeCell ref="B2:B14"/>
     <mergeCell ref="B15:B30"/>
     <mergeCell ref="B31:B42"/>
     <mergeCell ref="B43:B45"/>
     <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B48:B54"/>
-    <mergeCell ref="B55:B63"/>
-    <mergeCell ref="B64:B121"/>
-    <mergeCell ref="D69:D71"/>
-    <mergeCell ref="E69:E71"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="E72:E75"/>
-    <mergeCell ref="B122:B182"/>
-    <mergeCell ref="A183:B202"/>
-    <mergeCell ref="A203:B204"/>
-    <mergeCell ref="C203:C204"/>
+    <mergeCell ref="B48:B57"/>
+    <mergeCell ref="B58:B66"/>
+    <mergeCell ref="B67:B124"/>
+    <mergeCell ref="D72:D74"/>
+    <mergeCell ref="E72:E74"/>
+    <mergeCell ref="D75:D78"/>
+    <mergeCell ref="E75:E78"/>
+    <mergeCell ref="B125:B185"/>
+    <mergeCell ref="A186:B205"/>
+    <mergeCell ref="A206:B207"/>
+    <mergeCell ref="C206:C207"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>